<commit_message>
Correct Ak from ELOW (values below 5 = 0)
</commit_message>
<xml_diff>
--- a/Data/7. Covers/20230725_tiles_species_visual_census_25subquadrats.xlsx
+++ b/Data/7. Covers/20230725_tiles_species_visual_census_25subquadrats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremycarlot/Documents/Post-Doc – LOV/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/7. Covers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B596E7-49EB-6E45-BF3C-5597774420DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41036F5-DF77-264F-A780-1F69C0ABA2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="760" windowWidth="25440" windowHeight="13760" tabRatio="866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44120" yWindow="1060" windowWidth="40240" windowHeight="23080" tabRatio="866" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tile_02" sheetId="4" r:id="rId1"/>
@@ -2333,11 +2333,11 @@
   </sheetPr>
   <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15896,11 +15896,11 @@
   </sheetPr>
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21:XFD21"/>
+      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16545,15 +16545,6 @@
         <v>364</v>
       </c>
       <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
         <v>1</v>
       </c>
     </row>

</xml_diff>